<commit_message>
Updated phase 2 requirements partially, yet to implement
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Phase1" sheetId="1" r:id="rId1"/>
+    <sheet name="Phase2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>Not connected</t>
   </si>
@@ -102,6 +103,36 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>Notification</t>
+  </si>
+  <si>
+    <t>Do you want to monitor?</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Start monitoring</t>
+  </si>
+  <si>
+    <t>if Stopped throw Toast</t>
+  </si>
+  <si>
+    <t>Dismiss</t>
+  </si>
+  <si>
+    <t>No action</t>
+  </si>
+  <si>
+    <t>Alert</t>
+  </si>
+  <si>
+    <t>Max/min level reached</t>
+  </si>
+  <si>
+    <t>Stop monitoring</t>
   </si>
 </sst>
 </file>
@@ -421,7 +452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -566,4 +597,75 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Notification when plugged in and on alert
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
   <si>
     <t>Not connected</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t>Post Info on to main activity instead using Toasts</t>
+  </si>
+  <si>
+    <t>Memory</t>
+  </si>
+  <si>
+    <t>Store entered value in SharedPreferences</t>
   </si>
 </sst>
 </file>
@@ -613,86 +619,126 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="11" max="11" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="12" max="12" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>30</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1.2</v>
+      </c>
+      <c r="D3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>32</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
         <v>33</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2.1</v>
+      </c>
+      <c r="D6" t="s">
         <v>31</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
         <v>38</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>4.0999999999999996</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>